<commit_message>
Add validation of end point to logic
Correct some errors in input data file
</commit_message>
<xml_diff>
--- a/Vertices.xlsx
+++ b/Vertices.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,8 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11610"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$H$69</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="168">
   <si>
     <t>Vertex Name</t>
   </si>
@@ -270,6 +274,264 @@
   </si>
   <si>
     <t>V65</t>
+  </si>
+  <si>
+    <t>Vertex X_Width</t>
+  </si>
+  <si>
+    <t>Vertex Y_Height</t>
+  </si>
+  <si>
+    <t>RedStart</t>
+  </si>
+  <si>
+    <t>Red Null</t>
+  </si>
+  <si>
+    <t>Blue Null</t>
+  </si>
+  <si>
+    <t>RedPowerCube</t>
+  </si>
+  <si>
+    <t>RedSwitch</t>
+  </si>
+  <si>
+    <t>RedPlatformGap</t>
+  </si>
+  <si>
+    <t>RedPlatform</t>
+  </si>
+  <si>
+    <t>BluePlatform</t>
+  </si>
+  <si>
+    <t>BluePlatformGap</t>
+  </si>
+  <si>
+    <t>BlueSwitch</t>
+  </si>
+  <si>
+    <t>BluePowerCube</t>
+  </si>
+  <si>
+    <t>BlueStart</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>V7</t>
+  </si>
+  <si>
+    <t>V66</t>
+  </si>
+  <si>
+    <t>V67</t>
+  </si>
+  <si>
+    <t>V68</t>
+  </si>
+  <si>
+    <t>V2,V8,V9</t>
+  </si>
+  <si>
+    <t>V3,V8,V9,V10</t>
+  </si>
+  <si>
+    <t>V4,V9,V10,V11</t>
+  </si>
+  <si>
+    <t>V5,V10,V11,V12</t>
+  </si>
+  <si>
+    <t>V6,V11,V12,V13</t>
+  </si>
+  <si>
+    <t>V7,V12,V13,V14</t>
+  </si>
+  <si>
+    <t>V13,V14</t>
+  </si>
+  <si>
+    <t>V9,V15,V16</t>
+  </si>
+  <si>
+    <t>V10,V15,V16</t>
+  </si>
+  <si>
+    <t>V11,V16</t>
+  </si>
+  <si>
+    <t>V13,V17</t>
+  </si>
+  <si>
+    <t>V14,V17,V18</t>
+  </si>
+  <si>
+    <t>V34,V37,V38</t>
+  </si>
+  <si>
+    <t>V17,V18</t>
+  </si>
+  <si>
+    <t>V16,V19,V20</t>
+  </si>
+  <si>
+    <t>V18,V24,V25</t>
+  </si>
+  <si>
+    <t>V24,V25</t>
+  </si>
+  <si>
+    <t>V20,V26,V27</t>
+  </si>
+  <si>
+    <t>V21,V25,V27,V28</t>
+  </si>
+  <si>
+    <t>V22,V27,V28,V29</t>
+  </si>
+  <si>
+    <t>V23,V28,V29,V30</t>
+  </si>
+  <si>
+    <t>V24,V29,V30,V31</t>
+  </si>
+  <si>
+    <t>V25,V30,V31,V32</t>
+  </si>
+  <si>
+    <t>V31,V32</t>
+  </si>
+  <si>
+    <t>V27,V33,V34</t>
+  </si>
+  <si>
+    <t>V28,V33,V34</t>
+  </si>
+  <si>
+    <t>V31,V35</t>
+  </si>
+  <si>
+    <t>V35,V36</t>
+  </si>
+  <si>
+    <t>V32,V35,V36</t>
+  </si>
+  <si>
+    <t>V52,V55,V56</t>
+  </si>
+  <si>
+    <t>V37,V38,V39</t>
+  </si>
+  <si>
+    <t>V36,V41,V42,V43</t>
+  </si>
+  <si>
+    <t>V42,V43</t>
+  </si>
+  <si>
+    <t>V38,V44,V45</t>
+  </si>
+  <si>
+    <t>V39,V44,V45,V46</t>
+  </si>
+  <si>
+    <t>V40,V45,V46,V37</t>
+  </si>
+  <si>
+    <t>V41,V46,V47,V48</t>
+  </si>
+  <si>
+    <t>V42,V47,V48,V49</t>
+  </si>
+  <si>
+    <t>V43,V48,V49,V50</t>
+  </si>
+  <si>
+    <t>V49,V50</t>
+  </si>
+  <si>
+    <t>V45,V51,V52</t>
+  </si>
+  <si>
+    <t>V46,V51,V52</t>
+  </si>
+  <si>
+    <t>V47,V52</t>
+  </si>
+  <si>
+    <t>V29,V34</t>
+  </si>
+  <si>
+    <t>V50,V53,V54</t>
+  </si>
+  <si>
+    <t>V19,V20</t>
+  </si>
+  <si>
+    <t>V53,V54</t>
+  </si>
+  <si>
+    <t>V55,V56,V57</t>
+  </si>
+  <si>
+    <t>V60,V61</t>
+  </si>
+  <si>
+    <t>V54,V59,V60,V61</t>
+  </si>
+  <si>
+    <t>V56,V62,V63,V64</t>
+  </si>
+  <si>
+    <t>V58,V63,V64,V65</t>
+  </si>
+  <si>
+    <t>V59,V64,V65,V66</t>
+  </si>
+  <si>
+    <t>V60,V665,V66,V67</t>
+  </si>
+  <si>
+    <t>V61,V66,V67,V68</t>
+  </si>
+  <si>
+    <t>V67,V68</t>
+  </si>
+  <si>
+    <t>V57,V62,V63,V64</t>
   </si>
 </sst>
 </file>
@@ -621,10 +883,1827 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>98</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>98</v>
+      </c>
+      <c r="F3">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>85</v>
+      </c>
+      <c r="E4">
+        <v>98</v>
+      </c>
+      <c r="F4">
+        <v>54.5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>139.5</v>
+      </c>
+      <c r="E5">
+        <v>98</v>
+      </c>
+      <c r="F5">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>184.5</v>
+      </c>
+      <c r="E6">
+        <v>98</v>
+      </c>
+      <c r="F6">
+        <v>54.25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>238.75</v>
+      </c>
+      <c r="E7">
+        <v>98</v>
+      </c>
+      <c r="F7">
+        <v>55</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>294</v>
+      </c>
+      <c r="E8">
+        <v>98</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9">
+        <v>98</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10">
+        <v>98</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>42</v>
+      </c>
+      <c r="F10">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11">
+        <v>98</v>
+      </c>
+      <c r="D11">
+        <v>85</v>
+      </c>
+      <c r="E11">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>54.5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12">
+        <v>98</v>
+      </c>
+      <c r="D12">
+        <v>139.5</v>
+      </c>
+      <c r="E12">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>184.5</v>
+      </c>
+      <c r="E13">
+        <v>42</v>
+      </c>
+      <c r="F13">
+        <v>54.25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14">
+        <v>98</v>
+      </c>
+      <c r="D14">
+        <v>238.75</v>
+      </c>
+      <c r="E14">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <v>55</v>
+      </c>
+      <c r="G14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>98</v>
+      </c>
+      <c r="D15">
+        <v>294</v>
+      </c>
+      <c r="E15">
+        <v>42</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+      <c r="G15" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16">
+        <v>140</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>56</v>
+      </c>
+      <c r="F16">
+        <v>30</v>
+      </c>
+      <c r="G16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17">
+        <v>140</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <v>56</v>
+      </c>
+      <c r="F17">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18">
+        <v>140</v>
+      </c>
+      <c r="D18">
+        <v>238.75</v>
+      </c>
+      <c r="E18">
+        <v>56</v>
+      </c>
+      <c r="F18">
+        <v>55</v>
+      </c>
+      <c r="G18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19">
+        <v>140</v>
+      </c>
+      <c r="D19">
+        <v>294</v>
+      </c>
+      <c r="E19">
+        <v>56</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20">
+        <v>196</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>65.5</v>
+      </c>
+      <c r="F20">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21">
+        <v>196</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <v>65.5</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22">
+        <v>196</v>
+      </c>
+      <c r="D22">
+        <v>95.25</v>
+      </c>
+      <c r="E22">
+        <v>65.5</v>
+      </c>
+      <c r="F22">
+        <v>44.25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23">
+        <v>196</v>
+      </c>
+      <c r="D23">
+        <v>139.5</v>
+      </c>
+      <c r="E23">
+        <v>65.5</v>
+      </c>
+      <c r="F23">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24">
+        <v>196</v>
+      </c>
+      <c r="D24">
+        <v>184.5</v>
+      </c>
+      <c r="E24">
+        <v>65.5</v>
+      </c>
+      <c r="F24">
+        <v>44.25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25">
+        <v>196</v>
+      </c>
+      <c r="D25">
+        <v>228.75</v>
+      </c>
+      <c r="E25">
+        <v>65.5</v>
+      </c>
+      <c r="F25">
+        <v>65.25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26">
+        <v>196</v>
+      </c>
+      <c r="D26">
+        <v>294</v>
+      </c>
+      <c r="E26">
+        <v>65.5</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>97</v>
+      </c>
+      <c r="H26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27">
+        <v>261.5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>26.5</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28">
+        <v>261.5</v>
+      </c>
+      <c r="D28">
+        <v>30</v>
+      </c>
+      <c r="E28">
+        <v>26.5</v>
+      </c>
+      <c r="F28">
+        <v>65.25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29">
+        <v>261.5</v>
+      </c>
+      <c r="D29">
+        <v>95.25</v>
+      </c>
+      <c r="E29">
+        <v>54.25</v>
+      </c>
+      <c r="F29">
+        <v>44.25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30">
+        <v>261.5</v>
+      </c>
+      <c r="D30">
+        <v>139.5</v>
+      </c>
+      <c r="E30">
+        <v>54.25</v>
+      </c>
+      <c r="F30">
+        <v>45</v>
+      </c>
+      <c r="G30" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31">
+        <v>261.5</v>
+      </c>
+      <c r="D31">
+        <v>184.5</v>
+      </c>
+      <c r="E31">
+        <v>54.25</v>
+      </c>
+      <c r="F31">
+        <v>44.25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32">
+        <v>261.5</v>
+      </c>
+      <c r="D32">
+        <v>228.75</v>
+      </c>
+      <c r="E32">
+        <v>26.5</v>
+      </c>
+      <c r="F32">
+        <v>65.25</v>
+      </c>
+      <c r="G32" t="s">
+        <v>97</v>
+      </c>
+      <c r="H32" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33">
+        <v>261.5</v>
+      </c>
+      <c r="D33">
+        <v>294</v>
+      </c>
+      <c r="E33">
+        <v>26.5</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34">
+        <v>288</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>72</v>
+      </c>
+      <c r="F34">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35">
+        <v>288</v>
+      </c>
+      <c r="D35">
+        <v>30</v>
+      </c>
+      <c r="E35">
+        <v>72</v>
+      </c>
+      <c r="F35">
+        <v>65.25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36">
+        <v>288</v>
+      </c>
+      <c r="D36">
+        <v>238.75</v>
+      </c>
+      <c r="E36">
+        <v>72</v>
+      </c>
+      <c r="F36">
+        <v>55</v>
+      </c>
+      <c r="G36" t="s">
+        <v>98</v>
+      </c>
+      <c r="H36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37">
+        <v>288</v>
+      </c>
+      <c r="D37">
+        <v>294</v>
+      </c>
+      <c r="E37">
+        <v>72</v>
+      </c>
+      <c r="F37">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38">
+        <v>360</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>26.5</v>
+      </c>
+      <c r="F38">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39">
+        <v>360</v>
+      </c>
+      <c r="D39">
+        <v>30</v>
+      </c>
+      <c r="E39">
+        <v>26.5</v>
+      </c>
+      <c r="F39">
+        <v>65.25</v>
+      </c>
+      <c r="G39" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40">
+        <v>332.25</v>
+      </c>
+      <c r="D40">
+        <v>95.25</v>
+      </c>
+      <c r="E40">
+        <v>54.25</v>
+      </c>
+      <c r="F40">
+        <v>44.25</v>
+      </c>
+      <c r="G40" t="s">
+        <v>97</v>
+      </c>
+      <c r="H40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41">
+        <v>332.25</v>
+      </c>
+      <c r="D41">
+        <v>139.5</v>
+      </c>
+      <c r="E41">
+        <v>54.25</v>
+      </c>
+      <c r="F41">
+        <v>45</v>
+      </c>
+      <c r="G41" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42">
+        <v>332.25</v>
+      </c>
+      <c r="D42">
+        <v>184.5</v>
+      </c>
+      <c r="E42">
+        <v>54.25</v>
+      </c>
+      <c r="F42">
+        <v>44.25</v>
+      </c>
+      <c r="G42" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43">
+        <v>360</v>
+      </c>
+      <c r="D43">
+        <v>228.75</v>
+      </c>
+      <c r="E43">
+        <v>26.5</v>
+      </c>
+      <c r="F43">
+        <v>65.25</v>
+      </c>
+      <c r="G43" t="s">
+        <v>97</v>
+      </c>
+      <c r="H43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44">
+        <v>360</v>
+      </c>
+      <c r="D44">
+        <v>294</v>
+      </c>
+      <c r="E44">
+        <v>26.5</v>
+      </c>
+      <c r="F44">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>97</v>
+      </c>
+      <c r="H44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45">
+        <v>386.5</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>65.5</v>
+      </c>
+      <c r="F45">
+        <v>30</v>
+      </c>
+      <c r="G45" t="s">
+        <v>97</v>
+      </c>
+      <c r="H45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46">
+        <v>386.5</v>
+      </c>
+      <c r="D46">
+        <v>30</v>
+      </c>
+      <c r="E46">
+        <v>65.5</v>
+      </c>
+      <c r="F46">
+        <v>65.25</v>
+      </c>
+      <c r="G46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47">
+        <v>386.5</v>
+      </c>
+      <c r="D47">
+        <v>95.25</v>
+      </c>
+      <c r="E47">
+        <v>65.5</v>
+      </c>
+      <c r="F47">
+        <v>44.25</v>
+      </c>
+      <c r="G47" t="s">
+        <v>97</v>
+      </c>
+      <c r="H47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48">
+        <v>386.5</v>
+      </c>
+      <c r="D48">
+        <v>139.5</v>
+      </c>
+      <c r="E48">
+        <v>65.5</v>
+      </c>
+      <c r="F48">
+        <v>45</v>
+      </c>
+      <c r="G48" t="s">
+        <v>97</v>
+      </c>
+      <c r="H48" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49">
+        <v>386.5</v>
+      </c>
+      <c r="D49">
+        <v>184.5</v>
+      </c>
+      <c r="E49">
+        <v>65.5</v>
+      </c>
+      <c r="F49">
+        <v>44.25</v>
+      </c>
+      <c r="G49" t="s">
+        <v>97</v>
+      </c>
+      <c r="H49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50">
+        <v>386.5</v>
+      </c>
+      <c r="D50">
+        <v>228.75</v>
+      </c>
+      <c r="E50">
+        <v>65.5</v>
+      </c>
+      <c r="F50">
+        <v>65.25</v>
+      </c>
+      <c r="G50" t="s">
+        <v>97</v>
+      </c>
+      <c r="H50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51">
+        <v>386.5</v>
+      </c>
+      <c r="D51">
+        <v>294</v>
+      </c>
+      <c r="E51">
+        <v>65.5</v>
+      </c>
+      <c r="F51">
+        <v>30</v>
+      </c>
+      <c r="G51" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52">
+        <v>452</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>56</v>
+      </c>
+      <c r="F52">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>97</v>
+      </c>
+      <c r="H52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53">
+        <v>452</v>
+      </c>
+      <c r="D53">
+        <v>30</v>
+      </c>
+      <c r="E53">
+        <v>56</v>
+      </c>
+      <c r="F53">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s">
+        <v>97</v>
+      </c>
+      <c r="H53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54">
+        <v>452</v>
+      </c>
+      <c r="D54">
+        <v>238.75</v>
+      </c>
+      <c r="E54">
+        <v>56</v>
+      </c>
+      <c r="F54">
+        <v>55</v>
+      </c>
+      <c r="G54" t="s">
+        <v>97</v>
+      </c>
+      <c r="H54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55">
+        <v>452</v>
+      </c>
+      <c r="D55">
+        <v>294</v>
+      </c>
+      <c r="E55">
+        <v>56</v>
+      </c>
+      <c r="F55">
+        <v>30</v>
+      </c>
+      <c r="G55" t="s">
+        <v>97</v>
+      </c>
+      <c r="H55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56">
+        <v>508</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>42</v>
+      </c>
+      <c r="F56">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>97</v>
+      </c>
+      <c r="H56" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57">
+        <v>508</v>
+      </c>
+      <c r="D57">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>42</v>
+      </c>
+      <c r="F57">
+        <v>55</v>
+      </c>
+      <c r="G57" t="s">
+        <v>97</v>
+      </c>
+      <c r="H57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58">
+        <v>508</v>
+      </c>
+      <c r="D58">
+        <v>85</v>
+      </c>
+      <c r="E58">
+        <v>42</v>
+      </c>
+      <c r="F58">
+        <v>54.5</v>
+      </c>
+      <c r="G58" t="s">
+        <v>97</v>
+      </c>
+      <c r="H58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59">
+        <v>508</v>
+      </c>
+      <c r="D59">
+        <v>139.5</v>
+      </c>
+      <c r="E59">
+        <v>42</v>
+      </c>
+      <c r="F59">
+        <v>45</v>
+      </c>
+      <c r="G59" t="s">
+        <v>98</v>
+      </c>
+      <c r="H59" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60">
+        <v>508</v>
+      </c>
+      <c r="D60">
+        <v>184.5</v>
+      </c>
+      <c r="E60">
+        <v>42</v>
+      </c>
+      <c r="F60">
+        <v>54.25</v>
+      </c>
+      <c r="G60" t="s">
+        <v>97</v>
+      </c>
+      <c r="H60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61">
+        <v>508</v>
+      </c>
+      <c r="D61">
+        <v>238.75</v>
+      </c>
+      <c r="E61">
+        <v>42</v>
+      </c>
+      <c r="F61">
+        <v>55</v>
+      </c>
+      <c r="G61" t="s">
+        <v>97</v>
+      </c>
+      <c r="H61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62">
+        <v>508</v>
+      </c>
+      <c r="D62">
+        <v>294</v>
+      </c>
+      <c r="E62">
+        <v>42</v>
+      </c>
+      <c r="F62">
+        <v>30</v>
+      </c>
+      <c r="G62" t="s">
+        <v>97</v>
+      </c>
+      <c r="H62" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63">
+        <v>550</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>98</v>
+      </c>
+      <c r="F63">
+        <v>30</v>
+      </c>
+      <c r="G63" t="s">
+        <v>97</v>
+      </c>
+      <c r="H63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C64">
+        <v>550</v>
+      </c>
+      <c r="D64">
+        <v>30</v>
+      </c>
+      <c r="E64">
+        <v>98</v>
+      </c>
+      <c r="F64">
+        <v>55</v>
+      </c>
+      <c r="G64" t="s">
+        <v>97</v>
+      </c>
+      <c r="H64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65">
+        <v>550</v>
+      </c>
+      <c r="D65">
+        <v>85</v>
+      </c>
+      <c r="E65">
+        <v>98</v>
+      </c>
+      <c r="F65">
+        <v>54.5</v>
+      </c>
+      <c r="G65" t="s">
+        <v>97</v>
+      </c>
+      <c r="H65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66">
+        <v>550</v>
+      </c>
+      <c r="D66">
+        <v>139.5</v>
+      </c>
+      <c r="E66">
+        <v>98</v>
+      </c>
+      <c r="F66">
+        <v>45</v>
+      </c>
+      <c r="G66" t="s">
+        <v>97</v>
+      </c>
+      <c r="H66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67">
+        <v>550</v>
+      </c>
+      <c r="D67">
+        <v>184.5</v>
+      </c>
+      <c r="E67">
+        <v>98</v>
+      </c>
+      <c r="F67">
+        <v>54.25</v>
+      </c>
+      <c r="G67" t="s">
+        <v>97</v>
+      </c>
+      <c r="H67" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68">
+        <v>550</v>
+      </c>
+      <c r="D68">
+        <v>238.75</v>
+      </c>
+      <c r="E68">
+        <v>98</v>
+      </c>
+      <c r="F68">
+        <v>55</v>
+      </c>
+      <c r="G68" t="s">
+        <v>97</v>
+      </c>
+      <c r="H68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" t="s">
+        <v>95</v>
+      </c>
+      <c r="C69">
+        <v>550</v>
+      </c>
+      <c r="D69">
+        <v>294</v>
+      </c>
+      <c r="E69">
+        <v>98</v>
+      </c>
+      <c r="F69">
+        <v>30</v>
+      </c>
+      <c r="G69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H69"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B66"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>